<commit_message>
track generation code moved to project space in folder track_generation, best solution this far, pasts testing. Writing .wrl file commented out , not yet tested
</commit_message>
<xml_diff>
--- a/Simulationdata.xlsx
+++ b/Simulationdata.xlsx
@@ -103,7 +103,7 @@
     <col min="2" max="2" width="7.1796875" customWidth="true"/>
     <col min="3" max="3" width="22.453125" customWidth="true"/>
     <col min="4" max="4" width="11.453125" customWidth="true"/>
-    <col min="5" max="5" width="11.453125" customWidth="true"/>
+    <col min="5" max="5" width="10.453125" customWidth="true"/>
     <col min="6" max="6" width="13.453125" customWidth="true"/>
     <col min="7" max="7" width="11.81640625" customWidth="true"/>
     <col min="8" max="8" width="11.81640625" customWidth="true"/>
@@ -156,37 +156,37 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>6.7979371690258965</v>
+        <v>0.023917979180256017</v>
       </c>
       <c r="D2">
-        <v>54.277351713238609</v>
+        <v>60.175010850415752</v>
       </c>
       <c r="E2">
-        <v>97.709440062204379</v>
+        <v>100.46847197090533</v>
       </c>
       <c r="F2">
-        <v>0.016666895163400995</v>
+        <v>0.012710409572190263</v>
       </c>
       <c r="G2">
-        <v>60.520548108259</v>
+        <v>60.160343854906323</v>
       </c>
       <c r="H2">
-        <v>95.019747044920024</v>
+        <v>100.4495788777019</v>
       </c>
       <c r="I2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J2">
-        <v>5.9238157598078569</v>
+        <v>7.754907353445911</v>
       </c>
       <c r="K2">
-        <v>32.82</v>
+        <v>38.879999999999995</v>
       </c>
       <c r="L2">
-        <v>0.18049408165167144</v>
+        <v>0.19945749365858828</v>
       </c>
     </row>
     <row r="3">
@@ -194,37 +194,37 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>6.9072286760272146</v>
+        <v>0.017717331897139133</v>
       </c>
       <c r="D3">
-        <v>54.277351713238609</v>
+        <v>62.191760722286176</v>
       </c>
       <c r="E3">
-        <v>97.709440062204379</v>
+        <v>96.70264579205886</v>
       </c>
       <c r="F3">
-        <v>0.016666895163400995</v>
+        <v>0.0066459124260958838</v>
       </c>
       <c r="G3">
-        <v>60.365118422543979</v>
+        <v>62.179215652933962</v>
       </c>
       <c r="H3">
-        <v>94.446174140461878</v>
+        <v>96.690134793517515</v>
       </c>
       <c r="I3">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J3">
-        <v>3.8941354701074187</v>
+        <v>7.2129768560020224</v>
       </c>
       <c r="K3">
-        <v>32.82</v>
+        <v>38.159999999999997</v>
       </c>
       <c r="L3">
-        <v>0.11865129403130466</v>
+        <v>0.18901930964365887</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final solution- visualiser blocks in image processing are commented out to increase speed of simulation
</commit_message>
<xml_diff>
--- a/Simulationdata.xlsx
+++ b/Simulationdata.xlsx
@@ -104,7 +104,7 @@
     <col min="3" max="3" width="22.453125" customWidth="true"/>
     <col min="4" max="4" width="11.453125" customWidth="true"/>
     <col min="5" max="5" width="11.453125" customWidth="true"/>
-    <col min="6" max="6" width="15.453125" customWidth="true"/>
+    <col min="6" max="6" width="14.453125" customWidth="true"/>
     <col min="7" max="7" width="11.81640625" customWidth="true"/>
     <col min="8" max="8" width="11.81640625" customWidth="true"/>
     <col min="9" max="9" width="22.81640625" customWidth="true"/>
@@ -159,34 +159,34 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.017710544239862909</v>
+        <v>0.0028746441251000622</v>
       </c>
       <c r="D2">
-        <v>62.840394492103741</v>
+        <v>54.596546879440787</v>
       </c>
       <c r="E2">
-        <v>94.515436510201468</v>
+        <v>97.215001890946468</v>
       </c>
       <c r="F2">
-        <v>0.010830607957092474</v>
+        <v>0.0097316925231769966</v>
       </c>
       <c r="G2">
-        <v>62.847525123601443</v>
+        <v>54.598541370371024</v>
       </c>
       <c r="H2">
-        <v>94.499224864026075</v>
+        <v>97.212931725548444</v>
       </c>
       <c r="I2">
         <v>10</v>
       </c>
       <c r="J2">
-        <v>7.4787532043566625</v>
+        <v>8.3156501883134624</v>
       </c>
       <c r="K2">
-        <v>33.780000000000001</v>
+        <v>26.34</v>
       </c>
       <c r="L2">
-        <v>0.22139589118877034</v>
+        <v>0.31570425923741313</v>
       </c>
     </row>
     <row r="3">
@@ -197,34 +197,34 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.066106345565184271</v>
+        <v>0.034796800966771971</v>
       </c>
       <c r="D3">
-        <v>56.574968856701965</v>
+        <v>58.772891763598558</v>
       </c>
       <c r="E3">
-        <v>91.9940643772388</v>
+        <v>91.451446262207341</v>
       </c>
       <c r="F3">
-        <v>0.0034698971108332952</v>
+        <v>0.005465448303799394</v>
       </c>
       <c r="G3">
-        <v>56.634744628545448</v>
+        <v>58.774500592008572</v>
       </c>
       <c r="H3">
-        <v>91.965834853252389</v>
+        <v>91.416686673189801</v>
       </c>
       <c r="I3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J3">
-        <v>7.1951715329486268</v>
+        <v>4.4609972826772006</v>
       </c>
       <c r="K3">
-        <v>31.859999999999999</v>
+        <v>24.18</v>
       </c>
       <c r="L3">
-        <v>0.22583714792682444</v>
+        <v>0.18449120275753519</v>
       </c>
     </row>
     <row r="4">
@@ -235,34 +235,34 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.0051149663455797622</v>
+        <v>0.044388953645436859</v>
       </c>
       <c r="D4">
-        <v>59.436381291620471</v>
+        <v>54.398806760837324</v>
       </c>
       <c r="E4">
-        <v>93.061866604001025</v>
+        <v>98.676247774139767</v>
       </c>
       <c r="F4">
-        <v>0.014217321820481854</v>
+        <v>0.012292322976441174</v>
       </c>
       <c r="G4">
-        <v>59.436704867830287</v>
+        <v>54.426036646243276</v>
       </c>
       <c r="H4">
-        <v>93.06697132526206</v>
+        <v>98.641191925176784</v>
       </c>
       <c r="I4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J4">
-        <v>4.1183849815194762</v>
+        <v>4.7735435584867476</v>
       </c>
       <c r="K4">
-        <v>22.559999999999999</v>
+        <v>23.279999999999998</v>
       </c>
       <c r="L4">
-        <v>0.18255252577657255</v>
+        <v>0.20504912192812491</v>
       </c>
     </row>
     <row r="5">
@@ -273,34 +273,34 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0.039305883260359865</v>
+        <v>0.039782671942818003</v>
       </c>
       <c r="D5">
-        <v>59.173878091285232</v>
+        <v>58.465353255655756</v>
       </c>
       <c r="E5">
-        <v>96.756094437170773</v>
+        <v>91.735125369714851</v>
       </c>
       <c r="F5">
-        <v>0.00320987170066894</v>
+        <v>0.010993492743732071</v>
       </c>
       <c r="G5">
-        <v>59.189617534199407</v>
+        <v>58.46149370972757</v>
       </c>
       <c r="H5">
-        <v>96.720077463455198</v>
+        <v>91.774720380664945</v>
       </c>
       <c r="I5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J5">
-        <v>3.9017874885272432</v>
+        <v>4.1933899910015384</v>
       </c>
       <c r="K5">
-        <v>20.939999999999998</v>
+        <v>22.98</v>
       </c>
       <c r="L5">
-        <v>0.18633178073196005</v>
+        <v>0.18247998220198164</v>
       </c>
     </row>
     <row r="6">
@@ -311,34 +311,34 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0.042728857471647473</v>
+        <v>0.060366927351057698</v>
       </c>
       <c r="D6">
-        <v>61.795183913502157</v>
+        <v>59.100529481245289</v>
       </c>
       <c r="E6">
-        <v>93.418981178574683</v>
+        <v>96.690259622842319</v>
       </c>
       <c r="F6">
-        <v>0.011068719229711893</v>
+        <v>0.0054217613519634399</v>
       </c>
       <c r="G6">
-        <v>61.827955553148527</v>
+        <v>59.126009092997812</v>
       </c>
       <c r="H6">
-        <v>93.391562664834495</v>
+        <v>96.635533438042458</v>
       </c>
       <c r="I6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J6">
-        <v>5.4757136962533295</v>
+        <v>4.8775906055627996</v>
       </c>
       <c r="K6">
-        <v>28.919999999999998</v>
+        <v>25.02</v>
       </c>
       <c r="L6">
-        <v>0.18934003099077903</v>
+        <v>0.19494766608964029</v>
       </c>
     </row>
     <row r="7">
@@ -349,34 +349,34 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.060780286739798239</v>
+        <v>0.042166637796352796</v>
       </c>
       <c r="D7">
-        <v>55.749342224580964</v>
+        <v>55.491301405110399</v>
       </c>
       <c r="E7">
-        <v>97.75008836366753</v>
+        <v>100.90095272866</v>
       </c>
       <c r="F7">
-        <v>0.01235417392875025</v>
+        <v>0.0094082841072456649</v>
       </c>
       <c r="G7">
-        <v>55.801229673859673</v>
+        <v>55.510523788153861</v>
       </c>
       <c r="H7">
-        <v>97.718434993175251</v>
+        <v>100.8634224031461</v>
       </c>
       <c r="I7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J7">
-        <v>4.1622540815355951</v>
+        <v>9.8198569838403476</v>
       </c>
       <c r="K7">
-        <v>24.300000000000001</v>
+        <v>40.859999999999999</v>
       </c>
       <c r="L7">
-        <v>0.17128617619488046</v>
+        <v>0.24032934370632275</v>
       </c>
     </row>
     <row r="8">
@@ -387,34 +387,34 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>0.055447489258497469</v>
+        <v>0.065108089837966399</v>
       </c>
       <c r="D8">
-        <v>60.231042358689351</v>
+        <v>59.665653512452216</v>
       </c>
       <c r="E8">
-        <v>98.583271481054297</v>
+        <v>99.904863677191784</v>
       </c>
       <c r="F8">
-        <v>0.013580929211525187</v>
+        <v>0.017717788174410453</v>
       </c>
       <c r="G8">
-        <v>60.267695747525316</v>
+        <v>59.680812987424005</v>
       </c>
       <c r="H8">
-        <v>98.541666755939104</v>
+        <v>99.841545009478949</v>
       </c>
       <c r="I8">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J8">
-        <v>5.9712374278124773</v>
+        <v>6.923502840605023</v>
       </c>
       <c r="K8">
-        <v>29.34</v>
+        <v>33.060000000000002</v>
       </c>
       <c r="L8">
-        <v>0.20351865807131825</v>
+        <v>0.20942234847565103</v>
       </c>
     </row>
     <row r="9">
@@ -425,34 +425,34 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>0.02807743442231548</v>
+        <v>0.028136075293246667</v>
       </c>
       <c r="D9">
-        <v>63.272444190538124</v>
+        <v>58.324322291562673</v>
       </c>
       <c r="E9">
-        <v>91.980138830904821</v>
+        <v>99.771363338068028</v>
       </c>
       <c r="F9">
-        <v>0.0035952915790325333</v>
+        <v>0.0012197510095658015</v>
       </c>
       <c r="G9">
-        <v>63.293080529126378</v>
+        <v>58.340561071188269</v>
       </c>
       <c r="H9">
-        <v>91.9610998221751</v>
+        <v>99.748386376363342</v>
       </c>
       <c r="I9">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J9">
-        <v>11.005684542226348</v>
+        <v>5.9235796617259417</v>
       </c>
       <c r="K9">
-        <v>50.939999999999998</v>
+        <v>27.899999999999999</v>
       </c>
       <c r="L9">
-        <v>0.21605191484543282</v>
+        <v>0.2123146832159836</v>
       </c>
     </row>
     <row r="10">
@@ -463,34 +463,34 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>0.028422503709930109</v>
+        <v>0.040183229798248343</v>
       </c>
       <c r="D10">
-        <v>54.556975780785699</v>
+        <v>53.608643245084181</v>
       </c>
       <c r="E10">
-        <v>97.186405142897698</v>
+        <v>93.082329722856684</v>
       </c>
       <c r="F10">
-        <v>0.0077005053406454839</v>
+        <v>0.012354099024950544</v>
       </c>
       <c r="G10">
-        <v>54.569001562153453</v>
+        <v>53.639320322755339</v>
       </c>
       <c r="H10">
-        <v>97.160652098424549</v>
+        <v>93.056375747003713</v>
       </c>
       <c r="I10">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J10">
-        <v>6.8012959871443464</v>
+        <v>4.4387309099317838</v>
       </c>
       <c r="K10">
-        <v>29.939999999999998</v>
+        <v>25.259999999999998</v>
       </c>
       <c r="L10">
-        <v>0.2271641946273997</v>
+        <v>0.17572173040109992</v>
       </c>
     </row>
     <row r="11">
@@ -501,34 +501,34 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>0.044503810813518216</v>
+        <v>0.060964283434334049</v>
       </c>
       <c r="D11">
-        <v>60.568506398510053</v>
+        <v>57.506994801223847</v>
       </c>
       <c r="E11">
-        <v>95.989916388115645</v>
+        <v>98.676483014862512</v>
       </c>
       <c r="F11">
-        <v>0.015090503434892138</v>
+        <v>0.0066383050852709975</v>
       </c>
       <c r="G11">
-        <v>60.558249854394738</v>
+        <v>57.511010590743595</v>
       </c>
       <c r="H11">
-        <v>95.946610586197934</v>
+        <v>98.615651137617149</v>
       </c>
       <c r="I11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J11">
-        <v>4.9691276134805769</v>
+        <v>5.3995618916907402</v>
       </c>
       <c r="K11">
-        <v>24</v>
+        <v>27.539999999999999</v>
       </c>
       <c r="L11">
-        <v>0.20704698389502404</v>
+        <v>0.19606252330031737</v>
       </c>
     </row>
     <row r="12">
@@ -539,34 +539,34 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>0.051986713720518427</v>
+        <v>0.021780996639694197</v>
       </c>
       <c r="D12">
-        <v>60.193089730389453</v>
+        <v>62.779147900314172</v>
       </c>
       <c r="E12">
-        <v>99.762305967255259</v>
+        <v>98.956722952400227</v>
       </c>
       <c r="F12">
-        <v>0.0030622564597161442</v>
+        <v>0.018074702091656441</v>
       </c>
       <c r="G12">
-        <v>60.228101300757189</v>
+        <v>62.781291378791188</v>
       </c>
       <c r="H12">
-        <v>99.723876703095712</v>
+        <v>98.935047682744766</v>
       </c>
       <c r="I12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J12">
-        <v>7.1462435631385475</v>
+        <v>7.3679041768311038</v>
       </c>
       <c r="K12">
-        <v>34.259999999999998</v>
+        <v>34.5</v>
       </c>
       <c r="L12">
-        <v>0.20858854533387472</v>
+        <v>0.21356243990814794</v>
       </c>
     </row>
     <row r="13">
@@ -577,34 +577,34 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>0.073650148812843666</v>
+        <v>0.036204652358648018</v>
       </c>
       <c r="D13">
-        <v>61.834402712988371</v>
+        <v>60.900828606393915</v>
       </c>
       <c r="E13">
-        <v>94.266312553997309</v>
+        <v>94.620299876616187</v>
       </c>
       <c r="F13">
-        <v>0.010347887563135393</v>
+        <v>0.0048845328496319937</v>
       </c>
       <c r="G13">
-        <v>61.787799195706327</v>
+        <v>60.933791960112671</v>
       </c>
       <c r="H13">
-        <v>94.209282241030465</v>
+        <v>94.605326761909396</v>
       </c>
       <c r="I13">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J13">
-        <v>6.3759787519696891</v>
+        <v>5.2317883053689389</v>
       </c>
       <c r="K13">
-        <v>30.299999999999997</v>
+        <v>28.859999999999999</v>
       </c>
       <c r="L13">
-        <v>0.21042834164916469</v>
+        <v>0.1812816460626798</v>
       </c>
     </row>
     <row r="14">
@@ -615,34 +615,34 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>0.014033640166736087</v>
+        <v>0.021610089045236605</v>
       </c>
       <c r="D14">
-        <v>61.878848769415555</v>
+        <v>55.006865750646938</v>
       </c>
       <c r="E14">
-        <v>91.928662965753233</v>
+        <v>96.893747223610873</v>
       </c>
       <c r="F14">
-        <v>0.0061371540595933664</v>
+        <v>0.010319682317701777</v>
       </c>
       <c r="G14">
-        <v>61.881221077260001</v>
+        <v>55.024604344555833</v>
       </c>
       <c r="H14">
-        <v>91.914831291529893</v>
+        <v>96.881404685999897</v>
       </c>
       <c r="I14">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J14">
-        <v>7.439391695235364</v>
+        <v>3.4830508268682796</v>
       </c>
       <c r="K14">
-        <v>37.439999999999998</v>
+        <v>20.460000000000001</v>
       </c>
       <c r="L14">
-        <v>0.19870170126162834</v>
+        <v>0.17023708831223261</v>
       </c>
     </row>
     <row r="15">
@@ -653,34 +653,34 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>0.043455816020895488</v>
+        <v>0.052784228552667373</v>
       </c>
       <c r="D15">
-        <v>60.421926762974309</v>
+        <v>60.550863665206428</v>
       </c>
       <c r="E15">
-        <v>97.721763776669079</v>
+        <v>99.244210372126503</v>
       </c>
       <c r="F15">
-        <v>0.0072180061362724039</v>
+        <v>0.0032750871438628521</v>
       </c>
       <c r="G15">
-        <v>60.42264041553198</v>
+        <v>60.542120545586044</v>
       </c>
       <c r="H15">
-        <v>97.678313821018136</v>
+        <v>99.19215527974157</v>
       </c>
       <c r="I15">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J15">
-        <v>4.5059206956939342</v>
+        <v>8.2287061130503893</v>
       </c>
       <c r="K15">
-        <v>25.259999999999998</v>
+        <v>38.699999999999996</v>
       </c>
       <c r="L15">
-        <v>0.17838165857854055</v>
+        <v>0.21262806493670258</v>
       </c>
     </row>
     <row r="16">
@@ -691,34 +691,34 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>0.035200773166104954</v>
+        <v>0.012138114006187273</v>
       </c>
       <c r="D16">
-        <v>58.10518870331537</v>
+        <v>60.354238760729359</v>
       </c>
       <c r="E16">
-        <v>97.360316469021598</v>
+        <v>93.636217284636444</v>
       </c>
       <c r="F16">
-        <v>0.00099312855554561539</v>
+        <v>0.0098119319452137331</v>
       </c>
       <c r="G16">
-        <v>58.123197207954789</v>
+        <v>60.366348984586658</v>
       </c>
       <c r="H16">
-        <v>97.330071003375593</v>
+        <v>93.635394916255905</v>
       </c>
       <c r="I16">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J16">
-        <v>3.7950581002377843</v>
+        <v>4.3295048570036956</v>
       </c>
       <c r="K16">
-        <v>19.259999999999998</v>
+        <v>24.48</v>
       </c>
       <c r="L16">
-        <v>0.19704351506945922</v>
+        <v>0.17685885853773267</v>
       </c>
     </row>
     <row r="17">
@@ -729,34 +729,34 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>0.042235007934438303</v>
+        <v>0.04068926460446743</v>
       </c>
       <c r="D17">
-        <v>60.11971934116319</v>
+        <v>55.872264290880679</v>
       </c>
       <c r="E17">
-        <v>98.485714874350407</v>
+        <v>97.788435280961423</v>
       </c>
       <c r="F17">
-        <v>0.010606105180164607</v>
+        <v>0.011828078885584918</v>
       </c>
       <c r="G17">
-        <v>60.118453005897194</v>
+        <v>55.895350929882916</v>
       </c>
       <c r="H17">
-        <v>98.443498854994999</v>
+        <v>97.75492970898253</v>
       </c>
       <c r="I17">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J17">
-        <v>5.9325194598843209</v>
+        <v>3.3748424033396223</v>
       </c>
       <c r="K17">
-        <v>29.52</v>
+        <v>18.539999999999999</v>
       </c>
       <c r="L17">
-        <v>0.20096610636464501</v>
+        <v>0.18203033459221266</v>
       </c>
     </row>
     <row r="18">
@@ -767,34 +767,34 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>0.051564606994438045</v>
+        <v>0.022619173843685225</v>
       </c>
       <c r="D18">
-        <v>55.630387459394385</v>
+        <v>58.592784603202531</v>
       </c>
       <c r="E18">
-        <v>100.23495816076827</v>
+        <v>93.068223523442654</v>
       </c>
       <c r="F18">
-        <v>0.0024281936247212781</v>
+        <v>0.01104709076742301</v>
       </c>
       <c r="G18">
-        <v>55.646285265046551</v>
+        <v>58.604080914015917</v>
       </c>
       <c r="H18">
-        <v>100.18590544963079</v>
+        <v>93.048627085312773</v>
       </c>
       <c r="I18">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J18">
-        <v>6.9659284096576473</v>
+        <v>7.2077196530872483</v>
       </c>
       <c r="K18">
-        <v>32.939999999999998</v>
+        <v>39.299999999999997</v>
       </c>
       <c r="L18">
-        <v>0.21147323648019575</v>
+        <v>0.18340253570196563</v>
       </c>
     </row>
     <row r="19">
@@ -805,34 +805,34 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>0.05685209857639624</v>
+        <v>0.016375289774925743</v>
       </c>
       <c r="D19">
-        <v>56.985067949664341</v>
+        <v>58.736698014982736</v>
       </c>
       <c r="E19">
-        <v>94.552616269183076</v>
+        <v>92.485861247285428</v>
       </c>
       <c r="F19">
-        <v>0.0028033962695296908</v>
+        <v>0.013501795591147212</v>
       </c>
       <c r="G19">
-        <v>56.981687952920311</v>
+        <v>58.748390965304566</v>
       </c>
       <c r="H19">
-        <v>94.495864734097665</v>
+        <v>92.474397171745551</v>
       </c>
       <c r="I19">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J19">
-        <v>3.9046973164269416</v>
+        <v>3.2632196072322612</v>
       </c>
       <c r="K19">
-        <v>22.98</v>
+        <v>19.739999999999998</v>
       </c>
       <c r="L19">
-        <v>0.16991720262954488</v>
+        <v>0.16531001049808822</v>
       </c>
     </row>
     <row r="20">
@@ -843,34 +843,34 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>0.034338853272976866</v>
+        <v>0.0049847379363413963</v>
       </c>
       <c r="D20">
-        <v>56.109241668339962</v>
+        <v>62.218132829725278</v>
       </c>
       <c r="E20">
-        <v>90.768337326737438</v>
+        <v>94.132721010447653</v>
       </c>
       <c r="F20">
-        <v>0.0012743906131302061</v>
+        <v>0.0099254156560339823</v>
       </c>
       <c r="G20">
-        <v>56.142223717423057</v>
+        <v>62.214190955334068</v>
       </c>
       <c r="H20">
-        <v>90.777894590068712</v>
+        <v>94.129669905962729</v>
       </c>
       <c r="I20">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J20">
-        <v>5.1565753607520675</v>
+        <v>7.436528220818829</v>
       </c>
       <c r="K20">
-        <v>26.939999999999998</v>
+        <v>36.600000000000001</v>
       </c>
       <c r="L20">
-        <v>0.19140962734788672</v>
+        <v>0.20318383116991334</v>
       </c>
     </row>
     <row r="21">
@@ -881,34 +881,34 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>0.073193627175772311</v>
+        <v>0.022266557188626523</v>
       </c>
       <c r="D21">
-        <v>59.92666517529787</v>
+        <v>58.972601577717789</v>
       </c>
       <c r="E21">
-        <v>95.088956434652417</v>
+        <v>96.8369266734897</v>
       </c>
       <c r="F21">
-        <v>0.0045103612693984116</v>
+        <v>0.0050417693592628866</v>
       </c>
       <c r="G21">
-        <v>59.943300280840873</v>
+        <v>58.988766486965318</v>
       </c>
       <c r="H21">
-        <v>95.017678244981809</v>
+        <v>96.821613434836379</v>
       </c>
       <c r="I21">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J21">
-        <v>4.2531814078027557</v>
+        <v>4.9216470644687895</v>
       </c>
       <c r="K21">
-        <v>23.460000000000001</v>
+        <v>26.52</v>
       </c>
       <c r="L21">
-        <v>0.18129503017062043</v>
+        <v>0.18558246849429824</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
latest matlab script file - robust vs previous ones, not sure if simulink project is correct
</commit_message>
<xml_diff>
--- a/Simulationdata.xlsx
+++ b/Simulationdata.xlsx
@@ -13,27 +13,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Simulation no.</t>
   </si>
   <si>
+    <t>No. flights</t>
+  </si>
+  <si>
     <t>Success</t>
   </si>
   <si>
     <t>Distance from landing [m]</t>
   </si>
   <si>
+    <t>No. successful landings</t>
+  </si>
+  <si>
     <t>X distance error [m]</t>
   </si>
   <si>
     <t>Y distance error [m]</t>
   </si>
   <si>
+    <t>No. wrong landings/crashes</t>
+  </si>
+  <si>
     <t>X final [m]</t>
   </si>
   <si>
     <t>Y final [m]</t>
+  </si>
+  <si>
+    <t>No. timeouts (drone lost/confused)</t>
   </si>
   <si>
     <t>Z final [m]</t>
@@ -102,7 +114,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N5"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.90625" customWidth="true"/>
@@ -126,43 +138,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2">
@@ -173,40 +185,40 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.028257731645139141</v>
+        <v>0.04576081689766761</v>
       </c>
       <c r="D2">
-        <v>-0.017560679481888997</v>
+        <v>-0.030602637459161031</v>
       </c>
       <c r="E2">
-        <v>0.022138697655080364</v>
+        <v>0.034022506428613042</v>
       </c>
       <c r="F2">
-        <v>59.44204315260346</v>
+        <v>55.543235369244492</v>
       </c>
       <c r="G2">
-        <v>97.655006589443062</v>
+        <v>89.238759875282767</v>
       </c>
       <c r="H2">
-        <v>0.0060905404631734494</v>
+        <v>0.0093959223994030776</v>
       </c>
       <c r="I2">
-        <v>59.459603832085349</v>
+        <v>55.573838006703653</v>
       </c>
       <c r="J2">
-        <v>97.632867891787981</v>
+        <v>89.204737368854154</v>
       </c>
       <c r="K2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L2">
-        <v>8.3045496120832816</v>
+        <v>6.9567927375505398</v>
       </c>
       <c r="M2">
-        <v>41.280000000000001</v>
+        <v>32.939999999999998</v>
       </c>
       <c r="N2">
-        <v>0.20117610494387794</v>
+        <v>0.21119589367184397</v>
       </c>
     </row>
     <row r="3">
@@ -217,40 +229,66 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.0336314206608814</v>
+        <v>0.033424146466506821</v>
       </c>
       <c r="D3">
-        <v>-0.026560299566241952</v>
+        <v>-0.023015189182707729</v>
       </c>
       <c r="E3">
-        <v>0.020630631173588654</v>
+        <v>0.02423787601871652</v>
       </c>
       <c r="F3">
-        <v>53.230517782726466</v>
+        <v>59.680475767380941</v>
       </c>
       <c r="G3">
-        <v>92.024077143323083</v>
+        <v>91.68505240647508</v>
       </c>
       <c r="H3">
-        <v>0.016880402795452991</v>
+        <v>0.0012119600498582471</v>
       </c>
       <c r="I3">
-        <v>53.257078082292708</v>
+        <v>59.703490956563648</v>
       </c>
       <c r="J3">
-        <v>92.003446512149495</v>
+        <v>91.660814530456364</v>
       </c>
       <c r="K3">
+        <v>9</v>
+      </c>
+      <c r="L3">
+        <v>5.5003980775087058</v>
+      </c>
+      <c r="M3">
+        <v>28.739999999999998</v>
+      </c>
+      <c r="N3">
+        <v>0.19138476261338574</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L3">
-        <v>6.6648878235538103</v>
-      </c>
-      <c r="M3">
-        <v>34.920000000000002</v>
-      </c>
-      <c r="N3">
-        <v>0.19086162152215952</v>
+      <c r="H5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>